<commit_message>
Added solution and packing data for modelling section
Added solution and packing data to the moedlling section.
</commit_message>
<xml_diff>
--- a/Nitrogen fixation/da Silva, ME_16052430_CSC Data.xlsx
+++ b/Nitrogen fixation/da Silva, ME_16052430_CSC Data.xlsx
@@ -4,23 +4,33 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="-9765" yWindow="5715" windowWidth="17760" windowHeight="8790" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment 1" sheetId="1" r:id="rId1"/>
     <sheet name="Experiment 2" sheetId="2" r:id="rId2"/>
     <sheet name="Experiment 3" sheetId="3" r:id="rId3"/>
-    <sheet name="Control experiment 1" sheetId="4" r:id="rId4"/>
+    <sheet name="webpage" sheetId="5" r:id="rId4"/>
+    <sheet name="Control experiment 1" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Experiment 1'!$B$1:$Q$1</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="40">
   <si>
     <t>Sample 1</t>
   </si>
@@ -120,6 +130,27 @@
   <si>
     <t>time</t>
   </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Growth (OD600)</t>
+  </si>
+  <si>
+    <t>Ammonia</t>
+  </si>
+  <si>
+    <t>Biomass (cells/mL)</t>
+  </si>
+  <si>
+    <t>Biomass(g/L)</t>
+  </si>
+  <si>
+    <t>Biomass</t>
+  </si>
 </sst>
 </file>
 
@@ -210,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -224,6 +255,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -234,11 +266,89 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="hh:mm:ss;@"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -274,7 +384,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -384,6 +493,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D43B-4714-82C0-55433530E9A9}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -481,6 +595,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D43B-4714-82C0-55433530E9A9}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -578,6 +697,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-D43B-4714-82C0-55433530E9A9}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -675,6 +799,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-D43B-4714-82C0-55433530E9A9}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -772,6 +901,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-D43B-4714-82C0-55433530E9A9}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -869,6 +1003,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-D43B-4714-82C0-55433530E9A9}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -878,11 +1017,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="306096000"/>
-        <c:axId val="306114560"/>
+        <c:axId val="222882432"/>
+        <c:axId val="222884608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="306096000"/>
+        <c:axId val="222882432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -904,19 +1043,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="306114560"/>
+        <c:crossAx val="222884608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="306114560"/>
+        <c:axId val="222884608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -938,14 +1076,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="306096000"/>
+        <c:crossAx val="222882432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1015,7 +1152,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1112,6 +1248,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B08F-422E-BFB1-E26560DB0F91}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1200,6 +1341,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B08F-422E-BFB1-E26560DB0F91}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1209,11 +1355,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="305784320"/>
-        <c:axId val="306380800"/>
+        <c:axId val="231119872"/>
+        <c:axId val="231216640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="305784320"/>
+        <c:axId val="231119872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1235,19 +1381,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="306380800"/>
+        <c:crossAx val="231216640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="306380800"/>
+        <c:axId val="231216640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1269,21 +1414,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="305784320"/>
+        <c:crossAx val="231119872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1333,7 +1476,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1420,6 +1562,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3421-430D-841A-BEC4281BDCEB}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1499,6 +1646,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3421-430D-841A-BEC4281BDCEB}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1508,11 +1660,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="306403968"/>
-        <c:axId val="306418432"/>
+        <c:axId val="231247232"/>
+        <c:axId val="231261696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="306403968"/>
+        <c:axId val="231247232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1534,19 +1686,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="306418432"/>
+        <c:crossAx val="231261696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="306418432"/>
+        <c:axId val="231261696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1582,14 +1733,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="306403968"/>
+        <c:crossAx val="231247232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1718,6 +1868,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F8BD-492C-ACE8-12D7EEF5D603}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1794,6 +1949,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F8BD-492C-ACE8-12D7EEF5D603}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1870,6 +2030,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F8BD-492C-ACE8-12D7EEF5D603}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1946,6 +2111,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-F8BD-492C-ACE8-12D7EEF5D603}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -2022,6 +2192,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-F8BD-492C-ACE8-12D7EEF5D603}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -2098,6 +2273,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-F8BD-492C-ACE8-12D7EEF5D603}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2107,11 +2287,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="306869760"/>
-        <c:axId val="306871680"/>
+        <c:axId val="231371520"/>
+        <c:axId val="231373440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="306869760"/>
+        <c:axId val="231371520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2140,12 +2320,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="306871680"/>
+        <c:crossAx val="231373440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="306871680"/>
+        <c:axId val="231373440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2174,7 +2354,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="306869760"/>
+        <c:crossAx val="231371520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2313,6 +2493,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E95A-4088-8F27-7DC14A04EBFA}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2389,6 +2574,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E95A-4088-8F27-7DC14A04EBFA}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2468,6 +2658,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E95A-4088-8F27-7DC14A04EBFA}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -2547,6 +2742,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-E95A-4088-8F27-7DC14A04EBFA}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -2626,6 +2826,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-E95A-4088-8F27-7DC14A04EBFA}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -2705,6 +2910,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-E95A-4088-8F27-7DC14A04EBFA}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2714,11 +2924,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="306536448"/>
-        <c:axId val="306538368"/>
+        <c:axId val="231486976"/>
+        <c:axId val="231488896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="306536448"/>
+        <c:axId val="231486976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2747,12 +2957,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="306538368"/>
+        <c:crossAx val="231488896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="306538368"/>
+        <c:axId val="231488896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2781,7 +2991,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="306536448"/>
+        <c:crossAx val="231486976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2833,7 +3043,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2911,6 +3120,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1FB4-4CC3-A933-3E41EAE887CE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2981,6 +3195,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1FB4-4CC3-A933-3E41EAE887CE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -3051,6 +3270,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1FB4-4CC3-A933-3E41EAE887CE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -3121,6 +3345,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-1FB4-4CC3-A933-3E41EAE887CE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -3191,6 +3420,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-1FB4-4CC3-A933-3E41EAE887CE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -3261,6 +3495,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-1FB4-4CC3-A933-3E41EAE887CE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3270,11 +3509,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="306557696"/>
-        <c:axId val="306559616"/>
+        <c:axId val="233834752"/>
+        <c:axId val="234094976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="306557696"/>
+        <c:axId val="233834752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3296,19 +3535,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="m/d/yyyy\ h:mm" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="306559616"/>
+        <c:crossAx val="234094976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="306559616"/>
+        <c:axId val="234094976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3330,21 +3568,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="306557696"/>
+        <c:crossAx val="233834752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3458,6 +3694,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-30BB-46C6-979F-83BABB151073}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -3519,6 +3760,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-30BB-46C6-979F-83BABB151073}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -3580,6 +3826,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-30BB-46C6-979F-83BABB151073}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3589,11 +3840,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="306648192"/>
-        <c:axId val="306650112"/>
+        <c:axId val="234177280"/>
+        <c:axId val="234179200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="306648192"/>
+        <c:axId val="234177280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3622,12 +3873,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="306650112"/>
+        <c:crossAx val="234179200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="306650112"/>
+        <c:axId val="234179200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3656,7 +3907,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="306648192"/>
+        <c:crossAx val="234177280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3777,6 +4028,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B86C-43B3-B6D9-192672E184E8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -3838,6 +4094,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B86C-43B3-B6D9-192672E184E8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -3899,6 +4160,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B86C-43B3-B6D9-192672E184E8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3908,11 +4174,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="306685056"/>
-        <c:axId val="306686976"/>
+        <c:axId val="234207104"/>
+        <c:axId val="234221568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="306685056"/>
+        <c:axId val="234207104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3941,12 +4207,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="306686976"/>
+        <c:crossAx val="234221568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="306686976"/>
+        <c:axId val="234221568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3975,7 +4241,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="306685056"/>
+        <c:crossAx val="234207104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4027,7 +4293,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4096,6 +4361,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5C0F-4EC8-92C2-FED8D51D3738}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -4157,6 +4427,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5C0F-4EC8-92C2-FED8D51D3738}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -4218,6 +4493,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5C0F-4EC8-92C2-FED8D51D3738}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4227,11 +4507,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="306730112"/>
-        <c:axId val="306732032"/>
+        <c:axId val="234241024"/>
+        <c:axId val="234255488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="306730112"/>
+        <c:axId val="234241024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4253,19 +4533,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="m/d/yyyy\ h:mm" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="306732032"/>
+        <c:crossAx val="234255488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="306732032"/>
+        <c:axId val="234255488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4287,21 +4566,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="306730112"/>
+        <c:crossAx val="234241024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4333,7 +4610,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4368,7 +4651,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4398,7 +4687,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4433,7 +4728,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4463,7 +4764,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4493,7 +4800,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4528,7 +4841,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4558,7 +4877,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4588,7 +4913,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4604,6 +4935,66 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="D1:I67" totalsRowShown="0">
+  <autoFilter ref="D1:I67"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="date and time" dataDxfId="11"/>
+    <tableColumn id="2" name="Sample Number"/>
+    <tableColumn id="3" name="Description"/>
+    <tableColumn id="4" name="Juju"/>
+    <tableColumn id="5" name="Column1"/>
+    <tableColumn id="6" name="Column2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H9" totalsRowShown="0">
+  <autoFilter ref="A1:H9"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Time"/>
+    <tableColumn id="2" name="Growth (OD600)" dataDxfId="10"/>
+    <tableColumn id="3" name="pH" dataDxfId="9"/>
+    <tableColumn id="4" name="Ammonia"/>
+    <tableColumn id="5" name="Biomass (cells/mL)" dataDxfId="8">
+      <calculatedColumnFormula>4.9*10^7*B2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="Biomass(g/L)" dataDxfId="7">
+      <calculatedColumnFormula>2.464*B2+0.023</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="Biomass" dataDxfId="0">
+      <calculatedColumnFormula>(1000*Table2[[#This Row],[Biomass(g/L)]])/24.6</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" name="Glucose" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A1:G9" totalsRowShown="0">
+  <autoFilter ref="A1:G9"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Time"/>
+    <tableColumn id="2" name="Growth (OD600)" dataDxfId="6"/>
+    <tableColumn id="3" name="pH" dataDxfId="5"/>
+    <tableColumn id="4" name="Ammonia"/>
+    <tableColumn id="5" name="Biomass (cells/mL)" dataDxfId="4">
+      <calculatedColumnFormula>4.9*10^7*B2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="Biomass(g/L)" dataDxfId="3">
+      <calculatedColumnFormula>2.464*B2+0.023</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="Biomass" dataDxfId="2">
+      <calculatedColumnFormula>2.464*B2+0.023</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4896,7 +5287,7 @@
   <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="D1" sqref="D1:I67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4904,10 +5295,10 @@
     <col min="2" max="2" width="11.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
     <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.42578125" customWidth="1"/>
     <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4930,6 +5321,12 @@
       <c r="G1" t="s">
         <v>16</v>
       </c>
+      <c r="H1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -6534,6 +6931,9 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -6541,7 +6941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M3" sqref="M3:M10"/>
     </sheetView>
   </sheetViews>
@@ -6555,14 +6955,14 @@
       <c r="A1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13" t="s">
+      <c r="K1" s="14"/>
+      <c r="L1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="13"/>
+      <c r="M1" s="14"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
@@ -6900,12 +7300,12 @@
   <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3:S10"/>
+      <selection activeCell="D3" sqref="D3:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
@@ -6924,36 +7324,36 @@
       <c r="A1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14" t="s">
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14" t="s">
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14" t="s">
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14" t="s">
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
       <c r="T1" t="s">
         <v>15</v>
       </c>
@@ -7538,9 +7938,332 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5">
+        <v>5.2</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E9" si="0">4.9*10^7*B2</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ref="F2:F9" si="1">2.464*B2+0.023</f>
+        <v>2.3E-2</v>
+      </c>
+      <c r="G2">
+        <f>(1000*Table2[[#This Row],[Biomass(g/L)]])/24.6</f>
+        <v>0.93495934959349591</v>
+      </c>
+      <c r="H2" s="9">
+        <f>(5/30)*1000</f>
+        <v>166.66666666666666</v>
+      </c>
+      <c r="J2" s="13"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3" s="8">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f>4.9*10^7*B3</f>
+        <v>1225000</v>
+      </c>
+      <c r="F3">
+        <f>2.464*B3+0.023</f>
+        <v>8.4600000000000009E-2</v>
+      </c>
+      <c r="G3">
+        <f>(1000*Table2[[#This Row],[Biomass(g/L)]])/24.6</f>
+        <v>3.4390243902439024</v>
+      </c>
+      <c r="H3" s="9"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>23.5</v>
+      </c>
+      <c r="B4" s="8">
+        <v>1.3919999999999999</v>
+      </c>
+      <c r="C4" s="5">
+        <v>7.2</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>68208000</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>3.4528879999999997</v>
+      </c>
+      <c r="G4">
+        <f>(1000*Table2[[#This Row],[Biomass(g/L)]])/24.6</f>
+        <v>140.36130081300811</v>
+      </c>
+      <c r="H4" s="9">
+        <f>(((3.8*2)*(180.156)*(1/1000))/30)*1000</f>
+        <v>45.639520000000005</v>
+      </c>
+      <c r="J4" s="13"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>33.5</v>
+      </c>
+      <c r="B5" s="12">
+        <v>1.7283999999999999</v>
+      </c>
+      <c r="C5" s="5">
+        <v>7.3</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>84691600</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>4.2817775999999999</v>
+      </c>
+      <c r="G5">
+        <f>(1000*Table2[[#This Row],[Biomass(g/L)]])/24.6</f>
+        <v>174.05599999999995</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="8"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>47.5</v>
+      </c>
+      <c r="B6" s="12">
+        <v>1.9795</v>
+      </c>
+      <c r="C6" s="5">
+        <v>7.2</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>96995500</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>4.9004879999999993</v>
+      </c>
+      <c r="G6">
+        <f>(1000*Table2[[#This Row],[Biomass(g/L)]])/24.6</f>
+        <v>199.20682926829264</v>
+      </c>
+      <c r="H6" s="9">
+        <f>(((2.4)*(180.156)*(1/1000))/30)*1000</f>
+        <v>14.41248</v>
+      </c>
+      <c r="J6" s="13"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="8"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>52</v>
+      </c>
+      <c r="B7" s="12">
+        <v>2.0118</v>
+      </c>
+      <c r="C7" s="5">
+        <v>6.9</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f>4.9*10^7*B7</f>
+        <v>98578200</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>4.9800751999999999</v>
+      </c>
+      <c r="G7">
+        <f>(1000*Table2[[#This Row],[Biomass(g/L)]])/24.6</f>
+        <v>202.44208130081302</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="8"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>71.5</v>
+      </c>
+      <c r="B8" s="12">
+        <v>2.464</v>
+      </c>
+      <c r="C8" s="5">
+        <v>7.2</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>120736000</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>6.0942959999999999</v>
+      </c>
+      <c r="G8">
+        <f>(1000*Table2[[#This Row],[Biomass(g/L)]])/24.6</f>
+        <v>247.73560975609755</v>
+      </c>
+      <c r="H8" s="9">
+        <v>0</v>
+      </c>
+      <c r="J8" s="13"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>95.5</v>
+      </c>
+      <c r="B9" s="12">
+        <v>2.16</v>
+      </c>
+      <c r="C9" s="5">
+        <v>7.9</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>105840000</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>5.3452399999999995</v>
+      </c>
+      <c r="G9">
+        <f>(1000*Table2[[#This Row],[Biomass(g/L)]])/24.6</f>
+        <v>217.28617886178858</v>
+      </c>
+      <c r="H9" s="9">
+        <v>0</v>
+      </c>
+      <c r="J9" s="13"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
@@ -7556,21 +8279,21 @@
       <c r="A1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14" t="s">
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
       <c r="K1" t="s">
         <v>15</v>
       </c>
@@ -7862,4 +8585,259 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5">
+        <v>5.2</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E9" si="0">4.9*10^7*B2</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ref="F2:F9" si="1">2.464*B2+0.023</f>
+        <v>2.3E-2</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ref="G2:G9" si="2">2.464*B2+0.023</f>
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3" s="8">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>1225000</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="1"/>
+        <v>8.4600000000000009E-2</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="2"/>
+        <v>8.4600000000000009E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>23.5</v>
+      </c>
+      <c r="B4" s="8">
+        <v>1.3919999999999999</v>
+      </c>
+      <c r="C4" s="5">
+        <v>7.2</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>68208000</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>3.4528879999999997</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>3.4528879999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>33.5</v>
+      </c>
+      <c r="B5" s="12">
+        <v>1.7283999999999999</v>
+      </c>
+      <c r="C5" s="5">
+        <v>7.3</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>84691600</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>4.2817775999999999</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>4.2817775999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>47.5</v>
+      </c>
+      <c r="B6" s="12">
+        <v>1.9795</v>
+      </c>
+      <c r="C6" s="5">
+        <v>7.2</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>96995500</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>4.9004879999999993</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>4.9004879999999993</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>52</v>
+      </c>
+      <c r="B7" s="12">
+        <v>2.0118</v>
+      </c>
+      <c r="C7" s="5">
+        <v>6.9</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>98578200</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>4.9800751999999999</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>4.9800751999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>71.5</v>
+      </c>
+      <c r="B8" s="12">
+        <v>2.464</v>
+      </c>
+      <c r="C8" s="5">
+        <v>7.2</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>120736000</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>6.0942959999999999</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>6.0942959999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>95.5</v>
+      </c>
+      <c r="B9" s="12">
+        <v>2.16</v>
+      </c>
+      <c r="C9" s="5">
+        <v>7.9</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>105840000</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>5.3452399999999995</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>5.3452399999999995</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>